<commit_message>
Update of presentation and related
</commit_message>
<xml_diff>
--- a/scratchClientTutorial/UK---English/Part-0--Presentation/Costs of the board for Weekendschool Lesson 2 v0.1.xlsx
+++ b/scratchClientTutorial/UK---English/Part-0--Presentation/Costs of the board for Weekendschool Lesson 2 v0.1.xlsx
@@ -8,9 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="Eendplankje" sheetId="1" r:id="rId1"/>
-    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
-    <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Eendplankje!$A$1:$H$47</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -676,10 +677,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -691,7 +695,8 @@
     <col min="5" max="5" width="3.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="8" width="193.7109375" customWidth="1"/>
+    <col min="8" max="8" width="87.85546875" customWidth="1"/>
+    <col min="35" max="35" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25">
@@ -1460,37 +1465,11 @@
     <hyperlink ref="H23" r:id="rId9"/>
     <hyperlink ref="H22" r:id="rId10"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="65" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
   <legacyDrawing r:id="rId12"/>
   <oleObjects>
     <oleObject progId="Packager Shell-object" shapeId="1025" r:id="rId13"/>
   </oleObjects>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>